<commit_message>
Straight beams redesigned: modular buildup. SXx4, SXx2, SXx1 ok
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7245e009bcd34e4e/!_munka/Revolution/RevvyDemoKit/Structural parts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{09234830-67D4-4833-9BB5-8C918B3D85A0}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{39092586-7F4E-44DB-ACEB-F35FA4998F53}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="17320" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -417,7 +417,7 @@
     <t>CAD file</t>
   </si>
   <si>
-    <t>iam v1.0</t>
+    <t>iam v2.0</t>
   </si>
 </sst>
 </file>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
@@ -1184,7 +1184,9 @@
       <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1196,7 +1198,9 @@
       <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>

</xml_diff>

<commit_message>
SXx4, V, L, T shaped beams added
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{39092586-7F4E-44DB-ACEB-F35FA4998F53}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{56860B3A-E4F7-4F0E-8F20-97BA0DC3EEBB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="17320" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="131">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -932,808 +932,891 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="4" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="37.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" thickBot="1">
+    <row r="1" spans="1:7" ht="18.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" thickBot="1">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>130</v>
-      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1">
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" ht="16" thickBot="1">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" ht="16" thickBot="1">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="16" thickBot="1">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="16" thickBot="1">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" ht="16" thickBot="1">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="16" thickBot="1">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="16" thickBot="1">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="16" thickBot="1">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="16" thickBot="1">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="16" thickBot="1">
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" ht="16" thickBot="1">
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="16" thickBot="1">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" ht="16" thickBot="1">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="16" thickBot="1">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="7">
+        <v>7</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1">
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="7">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" ht="16" thickBot="1">
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="C21" s="7">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="16" thickBot="1">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="C22" s="7">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="16" thickBot="1">
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" ht="16" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="7">
+        <v>6</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" ht="16" thickBot="1">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="16" thickBot="1">
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" ht="16" thickBot="1">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" ht="16" thickBot="1">
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" ht="16" thickBot="1">
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" ht="16" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" ht="16" thickBot="1">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" ht="16" thickBot="1">
       <c r="A29" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" ht="16" thickBot="1">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" ht="16" thickBot="1">
       <c r="A30" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" ht="16" thickBot="1">
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" ht="16" thickBot="1">
       <c r="A31" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="8"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:6" ht="16" thickBot="1">
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" ht="16" thickBot="1">
       <c r="A32" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:6" ht="16" thickBot="1">
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" ht="16" thickBot="1">
       <c r="A33" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" thickBot="1">
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" ht="16" thickBot="1">
       <c r="A34" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" ht="16" thickBot="1">
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" ht="16" thickBot="1">
       <c r="A35" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:6" ht="16" thickBot="1">
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" ht="16" thickBot="1">
       <c r="A36" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6" ht="16" thickBot="1">
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="8"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:6" ht="16" thickBot="1">
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="8"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" ht="16" thickBot="1">
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
         <v>80</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" ht="16" thickBot="1">
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="8"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" ht="16" thickBot="1">
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="8"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" ht="16" thickBot="1">
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="8"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6" ht="16" thickBot="1">
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="8"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="1:6" ht="16" thickBot="1">
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="8"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="1:6" ht="16" thickBot="1">
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="8"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6" ht="16" thickBot="1">
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" ht="16" thickBot="1">
       <c r="A46" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="8"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:6" ht="16" thickBot="1">
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" ht="16" thickBot="1">
       <c r="A47" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="8"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:6" ht="16" thickBot="1">
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" ht="16" thickBot="1">
       <c r="A48" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="8"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
-    </row>
-    <row r="49" spans="1:6" ht="16" thickBot="1">
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" ht="16" thickBot="1">
       <c r="A49" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="8"/>
+      <c r="C49" s="7"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="1:6" ht="16" thickBot="1">
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" ht="16" thickBot="1">
       <c r="A50" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="8"/>
+      <c r="C50" s="7"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" ht="16" thickBot="1">
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" ht="16" thickBot="1">
       <c r="A51" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="8"/>
+      <c r="C51" s="7"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" ht="16" thickBot="1">
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" ht="16" thickBot="1">
       <c r="A52" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="8"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
-    </row>
-    <row r="53" spans="1:6" ht="16" thickBot="1">
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" ht="16" thickBot="1">
       <c r="A53" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="8"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
-    </row>
-    <row r="54" spans="1:6" ht="16" thickBot="1">
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" ht="16" thickBot="1">
       <c r="A54" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="8"/>
+      <c r="C54" s="7"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
-    </row>
-    <row r="55" spans="1:6" ht="16" thickBot="1">
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" ht="16" thickBot="1">
       <c r="A55" s="10" t="s">
         <v>112</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="8"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
-    </row>
-    <row r="56" spans="1:6" ht="16" thickBot="1">
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="1:7" ht="16" thickBot="1">
       <c r="A56" s="12" t="s">
         <v>114</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="8"/>
+      <c r="C56" s="13"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="1:6" ht="16" thickBot="1">
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" ht="16" thickBot="1">
       <c r="A57" s="12" t="s">
         <v>116</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="8"/>
+      <c r="C57" s="13"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
-    </row>
-    <row r="58" spans="1:6" ht="16" thickBot="1">
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" ht="16" thickBot="1">
       <c r="A58" s="12" t="s">
         <v>118</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="8"/>
+      <c r="C58" s="13"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="8"/>
+      <c r="G58" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="16" thickBot="1">
+    <row r="59" spans="1:7" ht="16" thickBot="1">
       <c r="A59" s="12" t="s">
         <v>121</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="8"/>
+      <c r="C59" s="13"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
-    </row>
-    <row r="60" spans="1:6" ht="16" thickBot="1">
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" ht="16" thickBot="1">
       <c r="A60" s="12" t="s">
         <v>123</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="8"/>
+      <c r="C60" s="13"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
-    </row>
-    <row r="61" spans="1:6" ht="16" thickBot="1">
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" ht="16" thickBot="1">
       <c r="A61" s="15" t="s">
         <v>125</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="8"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-    </row>
-    <row r="62" spans="1:6" ht="16" thickBot="1">
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="1:7" ht="16" thickBot="1">
       <c r="A62" s="15" t="s">
         <v>127</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="8"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Curved beam CB4H added
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{56860B3A-E4F7-4F0E-8F20-97BA0DC3EEBB}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A034C89A-8FD9-4645-B637-AD923325C6CC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="17320" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -417,7 +417,10 @@
     <t>CAD file</t>
   </si>
   <si>
-    <t>iam v2.0</t>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>v1,0</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
@@ -1330,7 +1333,9 @@
         <v>53</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>

</xml_diff>

<commit_message>
Some axles, round beams, connector pins added
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{CBB5886A-E1BD-4ACF-B96F-9AFE536D6BC7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A034C89A-8FD9-4645-B637-AD923325C6CC}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="6_{5F2CC224-8539-4E90-8B1E-2C2DC23B5D7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{2886675B-8D22-441E-BE80-1BACA7F28CBB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="17320" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21120" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="137">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -36,6 +36,9 @@
     <t>RRF Part #</t>
   </si>
   <si>
+    <t>CAD file</t>
+  </si>
+  <si>
     <t>Target SPEC</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
     <t>S2x1</t>
   </si>
   <si>
+    <t>v2.0</t>
+  </si>
+  <si>
     <t>must withstand the following forces…</t>
   </si>
   <si>
@@ -261,6 +267,9 @@
     <t>CP1x1</t>
   </si>
   <si>
+    <t>v1.0</t>
+  </si>
+  <si>
     <t>Connector Pins - CP2x1</t>
   </si>
   <si>
@@ -363,6 +372,18 @@
     <t>AXb3</t>
   </si>
   <si>
+    <t>Connector triangle CT3x3</t>
+  </si>
+  <si>
+    <t>CT3x3</t>
+  </si>
+  <si>
+    <t>Connector triangle CT2x2</t>
+  </si>
+  <si>
+    <t>CT2x2</t>
+  </si>
+  <si>
     <t>Washers - WashS</t>
   </si>
   <si>
@@ -414,20 +435,14 @@
     <t>RBm</t>
   </si>
   <si>
-    <t>CAD file</t>
-  </si>
-  <si>
-    <t>v2.0</t>
-  </si>
-  <si>
-    <t>v1,0</t>
+    <t>v1,0 - thicken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,8 +499,12 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,8 +517,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -567,11 +598,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -619,6 +661,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -935,17 +989,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
     <col min="4" max="5" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="37.1796875" bestFit="1" customWidth="1"/>
@@ -971,47 +1025,47 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1019,14 +1073,14 @@
     </row>
     <row r="5" spans="1:7" ht="16" thickBot="1">
       <c r="A5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -1034,14 +1088,14 @@
     </row>
     <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -1049,14 +1103,14 @@
     </row>
     <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -1064,14 +1118,14 @@
     </row>
     <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1079,14 +1133,14 @@
     </row>
     <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -1094,14 +1148,14 @@
     </row>
     <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1109,14 +1163,14 @@
     </row>
     <row r="11" spans="1:7" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1124,14 +1178,14 @@
     </row>
     <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1139,14 +1193,14 @@
     </row>
     <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1154,14 +1208,14 @@
     </row>
     <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1169,14 +1223,14 @@
     </row>
     <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1184,14 +1238,14 @@
     </row>
     <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1199,14 +1253,14 @@
     </row>
     <row r="17" spans="1:7" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1214,14 +1268,14 @@
     </row>
     <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1229,16 +1283,14 @@
     </row>
     <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="7">
-        <v>7</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1246,16 +1298,14 @@
     </row>
     <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="7">
-        <v>7</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1263,16 +1313,14 @@
     </row>
     <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="7">
-        <v>5</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1280,16 +1328,14 @@
     </row>
     <row r="22" spans="1:7" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="7">
-        <v>5</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1297,16 +1343,14 @@
     </row>
     <row r="23" spans="1:7" ht="16" thickBot="1">
       <c r="A23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="7">
-        <v>6</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1314,27 +1358,29 @@
     </row>
     <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
+      <c r="D24" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1342,101 +1388,115 @@
     </row>
     <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="16" thickBot="1">
       <c r="A28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
+      <c r="D28" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="16" thickBot="1">
       <c r="A29" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" ht="16" thickBot="1">
       <c r="A30" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
+      <c r="D30" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="16" thickBot="1">
       <c r="A31" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" ht="16" thickBot="1">
       <c r="A32" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="16" thickBot="1">
+    <row r="33" spans="1:7" ht="15.5">
       <c r="A33" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -1444,12 +1504,12 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="16" thickBot="1">
+    <row r="34" spans="1:7" ht="15.5">
       <c r="A34" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
@@ -1459,10 +1519,10 @@
     </row>
     <row r="35" spans="1:7" ht="16" thickBot="1">
       <c r="A35" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
@@ -1472,10 +1532,10 @@
     </row>
     <row r="36" spans="1:7" ht="16" thickBot="1">
       <c r="A36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
@@ -1485,49 +1545,55 @@
     </row>
     <row r="37" spans="1:7" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
+      <c r="D38" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
@@ -1537,10 +1603,10 @@
     </row>
     <row r="41" spans="1:7" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="8"/>
@@ -1550,49 +1616,55 @@
     </row>
     <row r="42" spans="1:7" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>90</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
+      <c r="D42" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
+      <c r="D43" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="8"/>
+      <c r="D44" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="8"/>
@@ -1600,77 +1672,87 @@
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="16" thickBot="1">
+    <row r="46" spans="1:7" ht="15.5">
       <c r="A46" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
+      <c r="D46" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="16" thickBot="1">
+    <row r="47" spans="1:7" ht="15.5">
       <c r="A47" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="8"/>
+      <c r="D47" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="16" thickBot="1">
+    <row r="48" spans="1:7" ht="15.5">
       <c r="A48" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="8"/>
+      <c r="D48" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="16" thickBot="1">
+    <row r="49" spans="1:7" ht="15.5">
       <c r="A49" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
+      <c r="D49" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="16" thickBot="1">
+    <row r="50" spans="1:7" ht="15.5">
       <c r="A50" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="8"/>
+      <c r="D50" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="16" thickBot="1">
+    <row r="51" spans="1:7" ht="15.5">
       <c r="A51" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="8"/>
@@ -1678,12 +1760,12 @@
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="16" thickBot="1">
+    <row r="52" spans="1:7" ht="15.5">
       <c r="A52" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>
@@ -1693,10 +1775,10 @@
     </row>
     <row r="53" spans="1:7" ht="16" thickBot="1">
       <c r="A53" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="8"/>
@@ -1706,10 +1788,10 @@
     </row>
     <row r="54" spans="1:7" ht="16" thickBot="1">
       <c r="A54" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
@@ -1718,58 +1800,52 @@
       <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="16" thickBot="1">
-      <c r="A55" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C55" s="11"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="7"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="16" thickBot="1">
-      <c r="A56" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B56" s="13" t="s">
+    <row r="56" spans="1:7" ht="15.5">
+      <c r="A56" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="13"/>
+      <c r="B56" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="7"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="16" thickBot="1">
-      <c r="A57" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" s="13" t="s">
+    <row r="57" spans="1:7" ht="15.5">
+      <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="13"/>
+      <c r="B57" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" s="7"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" ht="16" thickBot="1">
-      <c r="A58" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" s="13" t="s">
+      <c r="A58" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="13"/>
+      <c r="B58" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="11"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="14" t="s">
-        <v>120</v>
-      </c>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="16" thickBot="1">
       <c r="A59" s="12" t="s">
@@ -1798,30 +1874,74 @@
       <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" ht="16" thickBot="1">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="16"/>
+      <c r="C61" s="13"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
+      <c r="G61" s="14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="16" thickBot="1">
-      <c r="A62" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="16" t="s">
+      <c r="A62" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="16"/>
+      <c r="B62" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="13"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" ht="16" thickBot="1">
+      <c r="A63" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" ht="16" thickBot="1">
+      <c r="A64" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" ht="16" thickBot="1">
+      <c r="A65" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" spans="1:7" ht="15.5">
+      <c r="A66" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Connector triangles, boxes added
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="6_{5F2CC224-8539-4E90-8B1E-2C2DC23B5D7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{2886675B-8D22-441E-BE80-1BACA7F28CBB}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="6_{5F2CC224-8539-4E90-8B1E-2C2DC23B5D7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{17DD82A3-D79E-463B-B91A-4304B343B94D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21120" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
+    <workbookView xWindow="28800" yWindow="-16425" windowWidth="28800" windowHeight="15975" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="137">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -435,7 +435,7 @@
     <t>RBm</t>
   </si>
   <si>
-    <t>v1,0 - thicken</t>
+    <t>v1,0 - Should be thicken</t>
   </si>
 </sst>
 </file>
@@ -989,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection sqref="A1:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
@@ -1521,11 +1521,13 @@
       <c r="A35" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
+      <c r="D35" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -1534,21 +1536,23 @@
       <c r="A36" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
+      <c r="D36" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="8" t="s">
@@ -1560,10 +1564,10 @@
     </row>
     <row r="38" spans="1:7" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="8" t="s">
@@ -1575,10 +1579,10 @@
     </row>
     <row r="39" spans="1:7" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
@@ -1590,66 +1594,66 @@
     </row>
     <row r="40" spans="1:7" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
+      <c r="D40" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
+      <c r="D41" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="D42" s="8" t="s">
-        <v>136</v>
-      </c>
+      <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="8" t="s">
-        <v>136</v>
-      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="8" t="s">
@@ -1661,53 +1665,53 @@
     </row>
     <row r="45" spans="1:7" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="8"/>
+      <c r="D45" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.5">
+    <row r="46" spans="1:7" ht="16" thickBot="1">
       <c r="A46" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>98</v>
+        <v>93</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="8" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.5">
+    <row r="47" spans="1:7" ht="16" thickBot="1">
       <c r="A47" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="8" t="s">
-        <v>80</v>
-      </c>
+      <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" ht="15.5">
       <c r="A48" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>102</v>
+        <v>97</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="8" t="s">
@@ -1719,10 +1723,10 @@
     </row>
     <row r="49" spans="1:7" ht="15.5">
       <c r="A49" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="8" t="s">
@@ -1734,10 +1738,10 @@
     </row>
     <row r="50" spans="1:7" ht="15.5">
       <c r="A50" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="8" t="s">
@@ -1749,36 +1753,40 @@
     </row>
     <row r="51" spans="1:7" ht="15.5">
       <c r="A51" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
+      <c r="D51" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" ht="15.5">
       <c r="A52" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="C52" s="7"/>
-      <c r="D52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="16" thickBot="1">
+    <row r="53" spans="1:7" ht="15.5">
       <c r="A53" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="8"/>
@@ -1786,12 +1794,12 @@
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="16" thickBot="1">
+    <row r="54" spans="1:7" ht="15.5">
       <c r="A54" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="8"/>
@@ -1800,20 +1808,24 @@
       <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="16" thickBot="1">
-      <c r="A55" s="9"/>
-      <c r="B55" s="18"/>
+      <c r="A55" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>112</v>
+      </c>
       <c r="C55" s="7"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.5">
+    <row r="56" spans="1:7" ht="16" thickBot="1">
       <c r="A56" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="8"/>
@@ -1821,53 +1833,24 @@
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.5">
-      <c r="A57" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>118</v>
-      </c>
+    <row r="57" spans="1:7" ht="16" thickBot="1">
+      <c r="A57" s="9"/>
+      <c r="B57" s="18"/>
       <c r="C57" s="7"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="16" thickBot="1">
-      <c r="A58" s="10" t="s">
+    <row r="59" spans="1:7" ht="15" thickBot="1"/>
+    <row r="60" spans="1:7" ht="16" thickBot="1">
+      <c r="A60" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B60" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-    </row>
-    <row r="59" spans="1:7" ht="16" thickBot="1">
-      <c r="A59" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-    </row>
-    <row r="60" spans="1:7" ht="16" thickBot="1">
-      <c r="A60" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" s="13"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
@@ -1875,25 +1858,23 @@
     </row>
     <row r="61" spans="1:7" ht="16" thickBot="1">
       <c r="A61" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="14" t="s">
-        <v>127</v>
-      </c>
+      <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" ht="16" thickBot="1">
       <c r="A62" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="8"/>
@@ -1903,45 +1884,73 @@
     </row>
     <row r="63" spans="1:7" ht="16" thickBot="1">
       <c r="A63" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C63" s="13"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
+      <c r="G63" s="14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="16" thickBot="1">
-      <c r="A64" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C64" s="16"/>
+      <c r="A64" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="13"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" ht="16" thickBot="1">
-      <c r="A65" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" s="16"/>
+      <c r="A65" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="13"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.5">
-      <c r="A66" s="19"/>
+    <row r="66" spans="1:7" ht="16" thickBot="1">
+      <c r="A66" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" spans="1:7" ht="16" thickBot="1">
+      <c r="A67" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.5">
+      <c r="A68" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CC2x2 fixed, wedges, Axle beams added
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="6_{5F2CC224-8539-4E90-8B1E-2C2DC23B5D7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{17DD82A3-D79E-463B-B91A-4304B343B94D}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="6_{5F2CC224-8539-4E90-8B1E-2C2DC23B5D7C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{24AB6D9A-AE22-49DC-9DD2-09D32A0152AC}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-16425" windowWidth="28800" windowHeight="15975" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="27090" windowHeight="15910" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="137">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -992,7 +992,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection sqref="A1:D56"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
@@ -1495,11 +1495,13 @@
       <c r="A33" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>71</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
+      <c r="D33" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -1508,11 +1510,13 @@
       <c r="A34" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>73</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -1697,11 +1701,13 @@
       <c r="A47" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="17" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="8"/>
+      <c r="D47" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -1811,7 +1817,7 @@
       <c r="A55" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="17" t="s">
         <v>112</v>
       </c>
       <c r="C55" s="7"/>
@@ -1824,7 +1830,7 @@
       <c r="A56" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="17" t="s">
         <v>114</v>
       </c>
       <c r="C56" s="7"/>

</xml_diff>

<commit_message>
Colored parts, v214 STEP file generated
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{87FB0F81-3353-4C2A-AE93-3C91218C601A}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{F7C5BC25-FEC8-418B-8597-90083FDED0E5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
+    <workbookView xWindow="18060" yWindow="10800" windowWidth="18060" windowHeight="10800" activeTab="1" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600" xr2:uid="{EF99A69C-17B1-4350-A774-B0539ECD671F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sum" sheetId="1" r:id="rId1"/>
+    <sheet name="Color Codes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="158">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -457,6 +459,48 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>White - P 1-1 C</t>
+  </si>
+  <si>
+    <t>Copper - 7579 C</t>
+  </si>
+  <si>
+    <t>Silver - 649 C</t>
+  </si>
+  <si>
+    <t>Gold - 7563 C</t>
+  </si>
+  <si>
+    <t>Blue - 285 C</t>
+  </si>
+  <si>
+    <t>Red - 185 C</t>
+  </si>
+  <si>
+    <t>Black - Neutral Black C</t>
+  </si>
+  <si>
+    <t>Any color</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Blue</t>
   </si>
 </sst>
 </file>
@@ -525,7 +569,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,8 +594,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -630,11 +680,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -707,6 +770,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,1565 +1097,1854 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D57" sqref="A1:D57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="7" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="37.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" thickBot="1">
+    <row r="1" spans="1:10" ht="18.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
+      <c r="H1" s="2"/>
       <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="31.5" thickBot="1">
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="31.5" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="8">
         <v>897.51</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G3" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" thickBot="1">
+    <row r="4" spans="1:10" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="8">
         <v>1327.3150000000001</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G4" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" ht="16" thickBot="1">
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="16" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8">
+      <c r="E5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="8">
         <v>1757.1210000000001</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G5" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="8"/>
+      <c r="H5" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" ht="16" thickBot="1">
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8">
+      <c r="E6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="8">
         <v>2186.9259999999999</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="16" thickBot="1">
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="8">
         <v>3476.3420000000001</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" ht="16" thickBot="1">
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8">
+      <c r="E8" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="8">
         <v>5195.5619999999999</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G8" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" ht="16" thickBot="1">
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="8">
+      <c r="E9" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="8">
         <v>6914.7830000000004</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G9" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" ht="16" thickBot="1">
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8">
+      <c r="E10" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="8">
         <v>10353.225</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="16" thickBot="1">
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="8">
+      <c r="E11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="8">
         <v>3293.1419999999998</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G11" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="8"/>
+      <c r="H11" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1">
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8">
+      <c r="E12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" s="8">
         <v>4847.1620000000003</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H12" s="8"/>
+      <c r="H12" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" ht="16" thickBot="1">
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="8">
+      <c r="E13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="8">
         <v>6401.183</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G13" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" ht="16" thickBot="1">
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="8">
+      <c r="E14" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="8">
         <v>9509.2250000000004</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G14" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H14" s="8"/>
+      <c r="H14" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" ht="16" thickBot="1">
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="8">
+      <c r="E15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="8">
         <v>12617.267</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G15" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H15" s="8"/>
+      <c r="H15" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="16" thickBot="1">
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="8">
+      <c r="E16" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="8">
         <v>18833.349999999999</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G16" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H16" s="8"/>
+      <c r="H16" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" ht="16" thickBot="1">
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="8">
+      <c r="E17" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="8">
         <v>6365.183</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G17" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="16" thickBot="1">
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="8">
+      <c r="E18" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="8">
         <v>12250.867</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G18" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" ht="16" thickBot="1">
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="8">
+      <c r="E19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="8">
         <v>3040.1970000000001</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G19" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H19" s="8"/>
+      <c r="H19" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" ht="16" thickBot="1">
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="8">
+      <c r="E20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="8">
         <v>3036.489</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G20" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H20" s="8"/>
+      <c r="H20" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1">
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="8">
+      <c r="E21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="8">
         <v>2158.3809999999999</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G21" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H21" s="8"/>
+      <c r="H21" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1">
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="8">
+      <c r="E22" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="8">
         <v>2137.413</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G22" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H22" s="8"/>
+      <c r="H22" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" ht="16" thickBot="1">
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="8">
+      <c r="E23" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="8">
         <v>2588.1860000000001</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G23" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" ht="16" thickBot="1">
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="8">
+      <c r="E24" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="8">
         <v>2351.4119999999998</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G24" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="8"/>
+      <c r="H24" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" ht="16" thickBot="1">
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="8">
+      <c r="E25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="8">
         <v>3398.395</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G25" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H25" s="8"/>
+      <c r="H25" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" ht="16" thickBot="1">
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="16" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="8">
+      <c r="E26" s="7"/>
+      <c r="F26" s="8">
         <v>822.64200000000005</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G26" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="8"/>
+      <c r="H26" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" ht="16" thickBot="1">
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="8">
+      <c r="E27" s="7"/>
+      <c r="F27" s="8">
         <v>1264.4280000000001</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H27" s="8"/>
+      <c r="H27" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9" ht="16" thickBot="1">
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" ht="16" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="8">
+      <c r="E28" s="7"/>
+      <c r="F28" s="8">
         <v>1706.2149999999999</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G28" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H28" s="8"/>
+      <c r="H28" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" ht="16" thickBot="1">
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" ht="16" thickBot="1">
       <c r="A29" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="8">
+      <c r="E29" s="7"/>
+      <c r="F29" s="8">
         <v>2148.0010000000002</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G29" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H29" s="8"/>
+      <c r="H29" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9" ht="16" thickBot="1">
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" ht="16" thickBot="1">
       <c r="A30" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="8">
+      <c r="E30" s="7"/>
+      <c r="F30" s="8">
         <v>3915.1469999999999</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G30" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H30" s="8"/>
+      <c r="H30" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9" ht="16" thickBot="1">
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" ht="16" thickBot="1">
       <c r="A31" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="8">
+      <c r="E31" s="7"/>
+      <c r="F31" s="8">
         <v>5682.2929999999997</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G31" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H31" s="8"/>
+      <c r="H31" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:9" ht="16" thickBot="1">
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" ht="16" thickBot="1">
       <c r="A32" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="8">
+      <c r="E32" s="7"/>
+      <c r="F32" s="8">
         <v>7449.4390000000003</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G32" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="8"/>
+      <c r="H32" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="1:9" ht="16" thickBot="1">
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" ht="16" thickBot="1">
       <c r="A33" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="8">
+      <c r="E33" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="8">
         <v>4241.7740000000003</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G33" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H33" s="8"/>
+      <c r="H33" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9" ht="16" thickBot="1">
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" ht="16" thickBot="1">
       <c r="A34" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="17"/>
+      <c r="D34" s="22" t="s">
         <v>78</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>137</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>143</v>
+      <c r="F34" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="1:9" ht="16" thickBot="1">
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" ht="16" thickBot="1">
       <c r="A35" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="8">
+      <c r="E35" s="7"/>
+      <c r="F35" s="8">
         <v>1296.4770000000001</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G35" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H35" s="8"/>
+      <c r="H35" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" ht="16" thickBot="1">
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="8">
+      <c r="E36" s="7"/>
+      <c r="F36" s="8">
         <v>3467.8870000000002</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G36" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H36" s="8"/>
+      <c r="H36" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="1:9" ht="16" thickBot="1">
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="8">
+      <c r="E37" s="7"/>
+      <c r="F37" s="8">
         <v>3469.6109999999999</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G37" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H37" s="8"/>
+      <c r="H37" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9" ht="16" thickBot="1">
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="8">
+      <c r="E38" s="7"/>
+      <c r="F38" s="8">
         <v>2229.1190000000001</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G38" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H38" s="8"/>
+      <c r="H38" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="1:9" ht="16" thickBot="1">
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="8">
+      <c r="E39" s="7"/>
+      <c r="F39" s="8">
         <v>380.85500000000002</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G39" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H39" s="8"/>
+      <c r="H39" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I39" s="8"/>
-    </row>
-    <row r="40" spans="1:9" ht="16" thickBot="1">
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="8">
+      <c r="E40" s="7"/>
+      <c r="F40" s="8">
         <v>530.44100000000003</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G40" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H40" s="8"/>
+      <c r="H40" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9" ht="16" thickBot="1">
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
         <v>81</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="8">
+      <c r="E41" s="7"/>
+      <c r="F41" s="8">
         <v>680.02700000000004</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G41" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H41" s="8"/>
+      <c r="H41" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I41" s="8"/>
-    </row>
-    <row r="42" spans="1:9" ht="16" thickBot="1">
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="8"/>
+      <c r="C42" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="22"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="F42" s="8"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="8"/>
+      <c r="H42" s="7"/>
       <c r="I42" s="8"/>
-    </row>
-    <row r="43" spans="1:9" ht="16" thickBot="1">
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="8"/>
+      <c r="C43" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" s="22"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="F43" s="8"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="8"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="8"/>
-    </row>
-    <row r="44" spans="1:9" ht="16" thickBot="1">
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="8">
+      <c r="E44" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F44" s="8">
         <v>1227.1959999999999</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G44" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H44" s="8"/>
+      <c r="H44" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I44" s="8"/>
-    </row>
-    <row r="45" spans="1:9" ht="16" thickBot="1">
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
         <v>89</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="8">
+      <c r="E45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" s="8">
         <v>4843.8680000000004</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G45" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H45" s="8"/>
+      <c r="H45" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="1:9" ht="16" thickBot="1">
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="9" t="s">
         <v>91</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="8">
+      <c r="E46" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F46" s="8">
         <v>6677.0190000000002</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G46" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H46" s="8"/>
+      <c r="H46" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I46" s="8"/>
-    </row>
-    <row r="47" spans="1:9" ht="16" thickBot="1">
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="8">
+      <c r="E47" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" s="8">
         <v>5425.3469999999998</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G47" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H47" s="8"/>
+      <c r="H47" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="1:9" ht="16" thickBot="1">
+      <c r="J47" s="8"/>
+    </row>
+    <row r="48" spans="1:10" ht="16" thickBot="1">
       <c r="A48" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="8">
+      <c r="E48" s="7"/>
+      <c r="F48" s="8">
         <v>357.15300000000002</v>
       </c>
-      <c r="E48" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G48" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H48" s="8"/>
+      <c r="H48" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I48" s="8"/>
-    </row>
-    <row r="49" spans="1:9" ht="16" thickBot="1">
+      <c r="J48" s="8"/>
+    </row>
+    <row r="49" spans="1:10" ht="16" thickBot="1">
       <c r="A49" s="9" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="8">
+      <c r="E49" s="7"/>
+      <c r="F49" s="8">
         <v>496.404</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G49" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H49" s="8"/>
+      <c r="H49" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:9" ht="16" thickBot="1">
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10" ht="16" thickBot="1">
       <c r="A50" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="8">
+      <c r="E50" s="7"/>
+      <c r="F50" s="8">
         <v>418.59699999999998</v>
       </c>
-      <c r="E50" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G50" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="8"/>
+      <c r="H50" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I50" s="8"/>
-    </row>
-    <row r="51" spans="1:9" ht="16" thickBot="1">
+      <c r="J50" s="8"/>
+    </row>
+    <row r="51" spans="1:10" ht="16" thickBot="1">
       <c r="A51" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="8">
+      <c r="E51" s="7"/>
+      <c r="F51" s="8">
         <v>838.15499999999997</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G51" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H51" s="8"/>
+      <c r="H51" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I51" s="8"/>
-    </row>
-    <row r="52" spans="1:9" ht="16" thickBot="1">
+      <c r="J51" s="8"/>
+    </row>
+    <row r="52" spans="1:10" ht="16" thickBot="1">
       <c r="A52" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C52" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="8">
+      <c r="E52" s="7"/>
+      <c r="F52" s="8">
         <v>1677.269</v>
       </c>
-      <c r="E52" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G52" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H52" s="8"/>
+      <c r="H52" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I52" s="8"/>
-    </row>
-    <row r="53" spans="1:9" ht="16" thickBot="1">
+      <c r="J52" s="8"/>
+    </row>
+    <row r="53" spans="1:10" ht="16" thickBot="1">
       <c r="A53" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="8">
+      <c r="E53" s="7"/>
+      <c r="F53" s="8">
         <v>336.875</v>
       </c>
-      <c r="E53" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G53" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H53" s="8"/>
+      <c r="H53" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I53" s="8"/>
-    </row>
-    <row r="54" spans="1:9" ht="16" thickBot="1">
+      <c r="J53" s="8"/>
+    </row>
+    <row r="54" spans="1:10" ht="16" thickBot="1">
       <c r="A54" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="8">
+      <c r="E54" s="7"/>
+      <c r="F54" s="8">
         <v>494.12</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G54" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H54" s="8"/>
+      <c r="H54" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I54" s="8"/>
-    </row>
-    <row r="55" spans="1:9" ht="16" thickBot="1">
+      <c r="J54" s="8"/>
+    </row>
+    <row r="55" spans="1:10" ht="16" thickBot="1">
       <c r="A55" s="9" t="s">
         <v>134</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="8">
+      <c r="E55" s="7"/>
+      <c r="F55" s="8">
         <v>633.37099999999998</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G55" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8" t="s">
+      <c r="H55" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="16" thickBot="1">
+    <row r="56" spans="1:10" ht="16" thickBot="1">
       <c r="A56" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="8">
+      <c r="E56" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" s="8">
         <v>1452.922</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G56" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H56" s="8"/>
+      <c r="H56" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I56" s="8"/>
-    </row>
-    <row r="57" spans="1:9" ht="16" thickBot="1">
+      <c r="J56" s="8"/>
+    </row>
+    <row r="57" spans="1:10" ht="16" thickBot="1">
       <c r="A57" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="8">
+      <c r="E57" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" s="8">
         <v>2350.4319999999998</v>
       </c>
-      <c r="E57" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G57" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="H57" s="8"/>
+      <c r="H57" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I57" s="8"/>
-    </row>
-    <row r="58" spans="1:9" ht="16" thickBot="1">
+      <c r="J57" s="8"/>
+    </row>
+    <row r="58" spans="1:10" ht="16" thickBot="1">
       <c r="A58" s="9"/>
       <c r="B58" s="18"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="8"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="22"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
+      <c r="F58" s="8"/>
       <c r="G58" s="7"/>
-      <c r="H58" s="8"/>
+      <c r="H58" s="7"/>
       <c r="I58" s="8"/>
-    </row>
-    <row r="60" spans="1:9" ht="15" thickBot="1"/>
-    <row r="61" spans="1:9" ht="16" thickBot="1">
+      <c r="J58" s="8"/>
+    </row>
+    <row r="60" spans="1:10" ht="15" thickBot="1"/>
+    <row r="61" spans="1:10" ht="16" thickBot="1">
       <c r="A61" s="10" t="s">
         <v>117</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="8"/>
+      <c r="C61" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" s="22"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="F61" s="8"/>
       <c r="G61" s="11"/>
-      <c r="H61" s="8"/>
+      <c r="H61" s="11"/>
       <c r="I61" s="8"/>
-    </row>
-    <row r="62" spans="1:9" ht="16" thickBot="1">
+      <c r="J61" s="8"/>
+    </row>
+    <row r="62" spans="1:10" ht="16" thickBot="1">
       <c r="A62" s="12" t="s">
         <v>119</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="8"/>
+      <c r="C62" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="22"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="F62" s="8"/>
       <c r="G62" s="13"/>
-      <c r="H62" s="8"/>
+      <c r="H62" s="13"/>
       <c r="I62" s="8"/>
-    </row>
-    <row r="63" spans="1:9" ht="16" thickBot="1">
+      <c r="J62" s="8"/>
+    </row>
+    <row r="63" spans="1:10" ht="16" thickBot="1">
       <c r="A63" s="12" t="s">
         <v>121</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="8"/>
+      <c r="C63" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="22"/>
       <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
+      <c r="F63" s="8"/>
       <c r="G63" s="13"/>
-      <c r="H63" s="8"/>
+      <c r="H63" s="13"/>
       <c r="I63" s="8"/>
-    </row>
-    <row r="64" spans="1:9" ht="16" thickBot="1">
+      <c r="J63" s="8"/>
+    </row>
+    <row r="64" spans="1:10" ht="16" thickBot="1">
       <c r="A64" s="12" t="s">
         <v>123</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="8"/>
+      <c r="C64" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" s="22"/>
       <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
+      <c r="F64" s="8"/>
       <c r="G64" s="13"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="14" t="s">
+      <c r="H64" s="13"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="16" thickBot="1">
+    <row r="65" spans="1:10" ht="16" thickBot="1">
       <c r="A65" s="12" t="s">
         <v>126</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="8"/>
+      <c r="C65" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="22"/>
       <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
+      <c r="F65" s="8"/>
       <c r="G65" s="13"/>
-      <c r="H65" s="8"/>
+      <c r="H65" s="13"/>
       <c r="I65" s="8"/>
-    </row>
-    <row r="66" spans="1:9" ht="16" thickBot="1">
+      <c r="J65" s="8"/>
+    </row>
+    <row r="66" spans="1:10" ht="16" thickBot="1">
       <c r="A66" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="22"/>
-      <c r="D66" s="8"/>
+      <c r="C66" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="22"/>
       <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
+      <c r="F66" s="8"/>
       <c r="G66" s="13"/>
-      <c r="H66" s="8"/>
+      <c r="H66" s="13"/>
       <c r="I66" s="8"/>
-    </row>
-    <row r="67" spans="1:9" ht="16" thickBot="1">
+      <c r="J66" s="8"/>
+    </row>
+    <row r="67" spans="1:10" ht="16" thickBot="1">
       <c r="A67" s="15" t="s">
         <v>130</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="8"/>
+      <c r="C67" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D67" s="22"/>
       <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="F67" s="8"/>
       <c r="G67" s="16"/>
-      <c r="H67" s="8"/>
+      <c r="H67" s="16"/>
       <c r="I67" s="8"/>
-    </row>
-    <row r="68" spans="1:9" ht="16" thickBot="1">
+      <c r="J67" s="8"/>
+    </row>
+    <row r="68" spans="1:10" ht="16" thickBot="1">
       <c r="A68" s="15" t="s">
         <v>132</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="8"/>
+      <c r="C68" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" s="22"/>
       <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
+      <c r="F68" s="8"/>
       <c r="G68" s="16"/>
-      <c r="H68" s="8"/>
+      <c r="H68" s="16"/>
       <c r="I68" s="8"/>
-    </row>
-    <row r="69" spans="1:9" ht="15.5">
+      <c r="J68" s="8"/>
+    </row>
+    <row r="69" spans="1:10" ht="15.5">
       <c r="A69" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A129726C-7E62-40BB-A008-C28D27274ACE}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="24.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" thickBot="1">
+      <c r="A2" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1">
+      <c r="A3" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" thickBot="1">
+      <c r="A4" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4">
+        <v>198</v>
+      </c>
+      <c r="C4">
+        <v>83</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1">
+      <c r="A5" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5">
+        <v>213</v>
+      </c>
+      <c r="C5">
+        <v>154</v>
+      </c>
+      <c r="D5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1">
+      <c r="A6" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <v>230</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="A7" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7">
+        <v>236</v>
+      </c>
+      <c r="C7">
+        <v>236</v>
+      </c>
+      <c r="D7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1">
+      <c r="A8" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8">
+        <v>255</v>
+      </c>
+      <c r="C8">
+        <v>255</v>
+      </c>
+      <c r="D8">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D8">
+    <sortCondition ref="A2:A8"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pin related parts updated, Steps generated
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{F7C5BC25-FEC8-418B-8597-90083FDED0E5}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{8EB54618-A9BB-4D9F-B718-919B5A5B986A}"/>
   <bookViews>
-    <workbookView xWindow="18060" yWindow="10800" windowWidth="18060" windowHeight="10800" activeTab="1" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600" xr2:uid="{EF99A69C-17B1-4350-A774-B0539ECD671F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600" activeTab="1" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
+    <workbookView xWindow="1520" yWindow="0" windowWidth="18060" windowHeight="21600" xr2:uid="{EF99A69C-17B1-4350-A774-B0539ECD671F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sum" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="158">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -569,7 +569,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,12 +591,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -774,13 +768,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,8 +1090,8 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
@@ -1112,9 +1100,9 @@
     <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.90625" customWidth="1"/>
     <col min="4" max="4" width="8.90625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" customWidth="1"/>
-    <col min="7" max="8" width="12.1796875" customWidth="1"/>
+    <col min="5" max="6" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
     <col min="10" max="10" width="37.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1127,8 +1115,8 @@
       <c r="C1" s="2"/>
       <c r="D1" s="21"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1150,13 +1138,13 @@
         <v>140</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>4</v>
@@ -1181,11 +1169,11 @@
       <c r="E3" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="8">
         <v>897.51</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>141</v>
@@ -1211,11 +1199,11 @@
       <c r="E4" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="8">
         <v>1327.3150000000001</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>141</v>
@@ -1239,11 +1227,11 @@
       <c r="E5" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="8">
         <v>1757.1210000000001</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>141</v>
@@ -1267,11 +1255,11 @@
       <c r="E6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="8">
         <v>2186.9259999999999</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>141</v>
@@ -1295,11 +1283,11 @@
       <c r="E7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="8">
         <v>3476.3420000000001</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>141</v>
@@ -1323,11 +1311,11 @@
       <c r="E8" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="8">
         <v>5195.5619999999999</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>141</v>
@@ -1351,11 +1339,11 @@
       <c r="E9" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="8">
         <v>6914.7830000000004</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>141</v>
@@ -1379,11 +1367,11 @@
       <c r="E10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="8">
         <v>10353.225</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>141</v>
@@ -1407,11 +1395,11 @@
       <c r="E11" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="8">
         <v>3293.1419999999998</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>141</v>
@@ -1435,11 +1423,11 @@
       <c r="E12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="8">
         <v>4847.1620000000003</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>141</v>
@@ -1463,11 +1451,11 @@
       <c r="E13" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="8">
         <v>6401.183</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>141</v>
@@ -1491,11 +1479,11 @@
       <c r="E14" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="8">
         <v>9509.2250000000004</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>141</v>
@@ -1519,11 +1507,11 @@
       <c r="E15" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="8">
         <v>12617.267</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>141</v>
@@ -1547,11 +1535,11 @@
       <c r="E16" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="8">
         <v>18833.349999999999</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>141</v>
@@ -1575,11 +1563,11 @@
       <c r="E17" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="8">
         <v>6365.183</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>141</v>
@@ -1603,11 +1591,11 @@
       <c r="E18" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="8">
         <v>12250.867</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>141</v>
@@ -1631,11 +1619,11 @@
       <c r="E19" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="8">
         <v>3040.1970000000001</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>141</v>
@@ -1659,11 +1647,11 @@
       <c r="E20" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="8">
         <v>3036.489</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>141</v>
@@ -1687,11 +1675,11 @@
       <c r="E21" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="8">
         <v>2158.3809999999999</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>141</v>
@@ -1715,11 +1703,11 @@
       <c r="E22" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="8">
         <v>2137.413</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>141</v>
@@ -1743,11 +1731,11 @@
       <c r="E23" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="8">
         <v>2588.1860000000001</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>141</v>
@@ -1771,11 +1759,11 @@
       <c r="E24" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G24" s="8">
         <v>2351.4119999999998</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>141</v>
@@ -1799,11 +1787,11 @@
       <c r="E25" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="8">
         <v>3398.395</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>141</v>
@@ -1818,18 +1806,20 @@
       <c r="B26" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8">
-        <v>822.64200000000005</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>141</v>
+      <c r="E26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="8">
+        <v>829.39300000000003</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>141</v>
@@ -1844,18 +1834,20 @@
       <c r="B27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8">
-        <v>1264.4280000000001</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>141</v>
+      <c r="E27" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1271.18</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>141</v>
@@ -1870,18 +1862,20 @@
       <c r="B28" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8">
-        <v>1706.2149999999999</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>141</v>
+      <c r="E28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1712.9659999999999</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>141</v>
@@ -1896,18 +1890,20 @@
       <c r="B29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8">
-        <v>2148.0010000000002</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>141</v>
+      <c r="E29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="8">
+        <v>2154.7530000000002</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>141</v>
@@ -1922,18 +1918,20 @@
       <c r="B30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8">
-        <v>3915.1469999999999</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>141</v>
+      <c r="E30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" s="8">
+        <v>3921.8980000000001</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>141</v>
@@ -1948,18 +1946,20 @@
       <c r="B31" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8">
-        <v>5682.2929999999997</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>141</v>
+      <c r="E31" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="8">
+        <v>5689.0439999999999</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>141</v>
@@ -1974,18 +1974,20 @@
       <c r="B32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8">
-        <v>7449.4390000000003</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>141</v>
+      <c r="E32" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="8">
+        <v>7456.19</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>141</v>
@@ -2009,11 +2011,11 @@
       <c r="E33" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="8">
         <v>4241.7740000000003</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>141</v>
@@ -2035,11 +2037,11 @@
       <c r="E34" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="24" t="s">
         <v>137</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>143</v>
@@ -2056,18 +2058,20 @@
       <c r="B35" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="17" t="s">
         <v>149</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8">
-        <v>1296.4770000000001</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>141</v>
+      <c r="E35" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" s="8">
+        <v>1312.221</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>141</v>
@@ -2082,18 +2086,20 @@
       <c r="B36" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="17" t="s">
         <v>149</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8">
-        <v>3467.8870000000002</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>141</v>
+      <c r="E36" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" s="8">
+        <v>3499.375</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>141</v>
@@ -2108,18 +2114,20 @@
       <c r="B37" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="17" t="s">
         <v>149</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8">
-        <v>3469.6109999999999</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>141</v>
+      <c r="E37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="8">
+        <v>3493.933</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>141</v>
@@ -2134,18 +2142,20 @@
       <c r="B38" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="17" t="s">
         <v>149</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8">
-        <v>2229.1190000000001</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>141</v>
+      <c r="E38" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="8">
+        <v>2245.569</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>141</v>
@@ -2160,18 +2170,20 @@
       <c r="B39" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="17" t="s">
         <v>150</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8">
-        <v>380.85500000000002</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>141</v>
+      <c r="E39" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="8">
+        <v>387.60700000000003</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>141</v>
@@ -2186,18 +2198,20 @@
       <c r="B40" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="17" t="s">
         <v>146</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8">
-        <v>530.44100000000003</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>141</v>
+      <c r="E40" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G40" s="8">
+        <v>543.13800000000003</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>141</v>
@@ -2212,18 +2226,20 @@
       <c r="B41" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="17" t="s">
         <v>148</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8">
-        <v>680.02700000000004</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>141</v>
+      <c r="E41" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="8">
+        <v>698.66800000000001</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>141</v>
@@ -2238,13 +2254,13 @@
       <c r="B42" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="26" t="s">
         <v>145</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
       <c r="H42" s="7"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -2256,13 +2272,13 @@
       <c r="B43" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="26" t="s">
         <v>151</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
       <c r="H43" s="7"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -2283,11 +2299,11 @@
       <c r="E44" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="8">
         <v>1227.1959999999999</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>141</v>
@@ -2311,11 +2327,11 @@
       <c r="E45" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="8">
         <v>4843.8680000000004</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>141</v>
@@ -2339,11 +2355,11 @@
       <c r="E46" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="8">
         <v>6677.0190000000002</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>141</v>
@@ -2367,11 +2383,11 @@
       <c r="E47" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="8">
         <v>5425.3469999999998</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>141</v>
@@ -2386,18 +2402,20 @@
       <c r="B48" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="7"/>
-      <c r="F48" s="8">
-        <v>357.15300000000002</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>141</v>
+      <c r="E48" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G48" s="8">
+        <v>340.899</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>141</v>
@@ -2412,18 +2430,20 @@
       <c r="B49" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8">
-        <v>496.404</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>141</v>
+      <c r="E49" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="8">
+        <v>480.15</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>141</v>
@@ -2438,18 +2458,20 @@
       <c r="B50" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="8">
+      <c r="E50" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G50" s="8">
         <v>418.59699999999998</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>141</v>
@@ -2464,18 +2486,20 @@
       <c r="B51" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="8">
+      <c r="E51" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="8">
         <v>838.15499999999997</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>141</v>
@@ -2490,18 +2514,20 @@
       <c r="B52" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="8">
+      <c r="E52" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" s="8">
         <v>1677.269</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>141</v>
@@ -2516,18 +2542,20 @@
       <c r="B53" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="F53" s="8">
-        <v>336.875</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>141</v>
+      <c r="E53" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G53" s="8">
+        <v>340.07600000000002</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>141</v>
@@ -2542,18 +2570,20 @@
       <c r="B54" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E54" s="7"/>
-      <c r="F54" s="8">
-        <v>494.12</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>141</v>
+      <c r="E54" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="8">
+        <v>497.10199999999998</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>141</v>
@@ -2568,18 +2598,20 @@
       <c r="B55" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E55" s="7"/>
-      <c r="F55" s="8">
-        <v>633.37099999999998</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>141</v>
+      <c r="E55" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="8">
+        <v>636.35299999999995</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>141</v>
@@ -2605,11 +2637,11 @@
       <c r="E56" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G56" s="8">
         <v>1452.922</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>141</v>
@@ -2633,11 +2665,11 @@
       <c r="E57" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F57" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="8">
         <v>2350.4319999999998</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>141</v>
@@ -2651,8 +2683,8 @@
       <c r="C58" s="18"/>
       <c r="D58" s="22"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
       <c r="H58" s="7"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -2670,8 +2702,8 @@
       </c>
       <c r="D61" s="22"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="8"/>
       <c r="H61" s="11"/>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
@@ -2688,8 +2720,8 @@
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="8"/>
       <c r="H62" s="13"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -2706,8 +2738,8 @@
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="13"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="8"/>
       <c r="H63" s="13"/>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
@@ -2724,8 +2756,8 @@
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="13"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="8"/>
       <c r="H64" s="13"/>
       <c r="I64" s="8"/>
       <c r="J64" s="14" t="s">
@@ -2744,8 +2776,8 @@
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="13"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="8"/>
       <c r="H65" s="13"/>
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
@@ -2762,8 +2794,8 @@
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="13"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="8"/>
       <c r="H66" s="13"/>
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
@@ -2780,8 +2812,8 @@
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="16"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="8"/>
       <c r="H67" s="16"/>
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
@@ -2798,8 +2830,8 @@
       </c>
       <c r="D68" s="22"/>
       <c r="E68" s="16"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="8"/>
       <c r="H68" s="16"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
@@ -2821,7 +2853,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
update with final RFQ list
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{8EB54618-A9BB-4D9F-B718-919B5A5B986A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600" activeTab="1" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
-    <workbookView xWindow="1520" yWindow="0" windowWidth="18060" windowHeight="21600" xr2:uid="{EF99A69C-17B1-4350-A774-B0539ECD671F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600"/>
+    <workbookView xWindow="1515" yWindow="0" windowWidth="18060" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Sum" sheetId="1" r:id="rId1"/>
     <sheet name="Color Codes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sum!$A$2:$J$58</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="160">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -368,15 +370,9 @@
     <t>AXb3</t>
   </si>
   <si>
-    <t>Connector triangle CT3x3</t>
-  </si>
-  <si>
     <t>CT3x3</t>
   </si>
   <si>
-    <t>Connector triangle CT2x2</t>
-  </si>
-  <si>
     <t>CT2x2</t>
   </si>
   <si>
@@ -501,13 +497,25 @@
   </si>
   <si>
     <t>Blue</t>
+  </si>
+  <si>
+    <t>S4x3</t>
+  </si>
+  <si>
+    <t>Straight Beams - S4x3</t>
+  </si>
+  <si>
+    <t>Connector Triangle CT3x3</t>
+  </si>
+  <si>
+    <t>Connector Triangle CT2x2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,8 +576,15 @@
       <sz val="12"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,6 +606,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -769,6 +790,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1084,30 +1117,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
-  <dimension ref="A1:J69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.5" thickBot="1">
+    <row r="1" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,7 +1154,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="31.5" thickBot="1">
+    <row r="2" spans="1:10" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1129,22 +1162,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>4</v>
@@ -1153,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" thickBot="1">
+    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1161,29 +1194,29 @@
         <v>7</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G3" s="8">
         <v>897.51</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1">
+    <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1191,27 +1224,27 @@
         <v>11</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G4" s="8">
         <v>1327.3150000000001</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="16" thickBot="1">
+    <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1219,27 +1252,27 @@
         <v>13</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G5" s="8">
         <v>1757.1210000000001</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="16" thickBot="1">
+    <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1247,27 +1280,27 @@
         <v>15</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G6" s="8">
         <v>2186.9259999999999</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="16" thickBot="1">
+    <row r="7" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -1275,27 +1308,27 @@
         <v>17</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G7" s="8">
         <v>3476.3420000000001</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="16" thickBot="1">
+    <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1303,27 +1336,27 @@
         <v>19</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G8" s="8">
         <v>5195.5619999999999</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="16" thickBot="1">
+    <row r="9" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1331,55 +1364,57 @@
         <v>21</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G9" s="8">
         <v>6914.7830000000004</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="16" thickBot="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>145</v>
+      <c r="C10" s="28" t="s">
+        <v>143</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G10" s="8">
         <v>10353.225</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="I10" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="16" thickBot="1">
+    <row r="11" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
@@ -1387,27 +1422,27 @@
         <v>25</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G11" s="8">
         <v>3293.1419999999998</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="16" thickBot="1">
+    <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
@@ -1415,27 +1450,27 @@
         <v>27</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G12" s="8">
         <v>4847.1620000000003</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1">
+    <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
@@ -1443,27 +1478,27 @@
         <v>29</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G13" s="8">
         <v>6401.183</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="16" thickBot="1">
+    <row r="14" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
@@ -1471,27 +1506,27 @@
         <v>31</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G14" s="8">
         <v>9509.2250000000004</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="16" thickBot="1">
+    <row r="15" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
@@ -1499,27 +1534,27 @@
         <v>33</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G15" s="8">
         <v>12617.267</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="16" thickBot="1">
+    <row r="16" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>34</v>
       </c>
@@ -1527,540 +1562,540 @@
         <v>35</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G16" s="8">
         <v>18833.349999999999</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="16" thickBot="1">
+    <row r="17" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G17" s="8">
-        <v>6365.183</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>141</v>
+      <c r="E17" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="29">
+        <v>4829.1620000000003</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>139</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="16" thickBot="1">
+    <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G18" s="8">
-        <v>12250.867</v>
+        <v>6365.183</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="16" thickBot="1">
+    <row r="19" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G19" s="8">
-        <v>3040.1970000000001</v>
+        <v>12250.867</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="16" thickBot="1">
+    <row r="20" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G20" s="8">
-        <v>3036.489</v>
+        <v>3040.1970000000001</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="16" thickBot="1">
+    <row r="21" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G21" s="8">
-        <v>2158.3809999999999</v>
+        <v>3036.489</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="16" thickBot="1">
+    <row r="22" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G22" s="8">
-        <v>2137.413</v>
+        <v>2158.3809999999999</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="16" thickBot="1">
+    <row r="23" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G23" s="8">
-        <v>2588.1860000000001</v>
+        <v>2137.413</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="16" thickBot="1">
-      <c r="A24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>146</v>
+    <row r="24" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>143</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G24" s="8">
-        <v>2351.4119999999998</v>
+        <v>2588.1860000000001</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="I24" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="16" thickBot="1">
+    <row r="25" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G25" s="8">
-        <v>3398.395</v>
+        <v>2351.4119999999998</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="16" thickBot="1">
+    <row r="26" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G26" s="8">
-        <v>829.39300000000003</v>
+        <v>3398.395</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="16" thickBot="1">
+    <row r="27" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G27" s="8">
-        <v>1271.18</v>
+        <v>829.39300000000003</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="16" thickBot="1">
+    <row r="28" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G28" s="8">
-        <v>1712.9659999999999</v>
+        <v>1271.18</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" ht="16" thickBot="1">
+    <row r="29" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G29" s="8">
-        <v>2154.7530000000002</v>
+        <v>1712.9659999999999</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" ht="16" thickBot="1">
+    <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G30" s="8">
-        <v>3921.8980000000001</v>
+        <v>2154.7530000000002</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" ht="16" thickBot="1">
+    <row r="31" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G31" s="8">
-        <v>5689.0439999999999</v>
+        <v>3921.8980000000001</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="16" thickBot="1">
+    <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G32" s="8">
-        <v>7456.19</v>
+        <v>5689.0439999999999</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="16" thickBot="1">
+    <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G33" s="8">
-        <v>4241.7740000000003</v>
+        <v>7456.19</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="16" thickBot="1">
+    <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="17"/>
+        <v>69</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>146</v>
+      </c>
       <c r="D34" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="24" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="G34" s="8">
+        <v>4241.7740000000003</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>137</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="I34" s="8"/>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="16" thickBot="1">
-      <c r="A35" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>149</v>
-      </c>
+    <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="28"/>
       <c r="D35" s="22" t="s">
         <v>78</v>
       </c>
@@ -2070,210 +2105,224 @@
       <c r="F35" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G35" s="8">
-        <v>1312.221</v>
+      <c r="G35" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="I35" s="8"/>
+      <c r="I35" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" ht="16" thickBot="1">
-      <c r="A36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>149</v>
+    <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>147</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G36" s="8">
-        <v>3499.375</v>
+        <v>3493.933</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="I36" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" ht="16" thickBot="1">
+    <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>114</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G37" s="8">
-        <v>3493.933</v>
+        <v>2245.569</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="16" thickBot="1">
+    <row r="38" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G38" s="8">
-        <v>2245.569</v>
+        <v>1312.221</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="16" thickBot="1">
+    <row r="39" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G39" s="8">
-        <v>387.60700000000003</v>
+        <v>3499.375</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="16" thickBot="1">
+    <row r="40" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G40" s="8">
-        <v>543.13800000000003</v>
+        <v>387.60700000000003</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="16" thickBot="1">
+    <row r="41" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G41" s="8">
-        <v>698.66800000000001</v>
+        <v>543.13800000000003</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" ht="16" thickBot="1">
+    <row r="42" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" s="8">
+        <v>698.66800000000001</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="16" thickBot="1">
+    <row r="43" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="7"/>
@@ -2283,458 +2332,460 @@
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="1:10" ht="16" thickBot="1">
+    <row r="44" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G44" s="8">
-        <v>1227.1959999999999</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="7"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10" ht="16" thickBot="1">
+    <row r="45" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G45" s="8">
-        <v>4843.8680000000004</v>
+        <v>1227.1959999999999</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:10" ht="16" thickBot="1">
+    <row r="46" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G46" s="8">
-        <v>6677.0190000000002</v>
+        <v>4843.8680000000004</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10" ht="16" thickBot="1">
+    <row r="47" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G47" s="8">
-        <v>5425.3469999999998</v>
+        <v>6677.0190000000002</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="16" thickBot="1">
+    <row r="48" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G48" s="8">
-        <v>340.899</v>
+        <v>5425.3469999999998</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10" ht="16" thickBot="1">
+    <row r="49" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G49" s="8">
-        <v>480.15</v>
+        <v>340.899</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="1:10" ht="16" thickBot="1">
+    <row r="50" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G50" s="8">
-        <v>418.59699999999998</v>
+        <v>480.15</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10" ht="16" thickBot="1">
+    <row r="51" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G51" s="8">
-        <v>838.15499999999997</v>
+        <v>418.59699999999998</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:10" ht="16" thickBot="1">
+    <row r="52" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G52" s="8">
-        <v>1677.269</v>
+        <v>838.15499999999997</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="1:10" ht="16" thickBot="1">
+    <row r="53" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G53" s="8">
-        <v>340.07600000000002</v>
+        <v>1677.269</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10" ht="16" thickBot="1">
+    <row r="54" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G54" s="8">
-        <v>497.10199999999998</v>
+        <v>340.07600000000002</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="1:10" ht="16" thickBot="1">
-      <c r="A55" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>151</v>
+    <row r="55" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>149</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G55" s="8">
-        <v>636.35299999999995</v>
+        <v>497.10199999999998</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="16" thickBot="1">
+        <v>139</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G56" s="8">
-        <v>1452.922</v>
+        <v>636.35299999999995</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="1:10" ht="16" thickBot="1">
+      <c r="J56" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G57" s="8">
-        <v>2350.4319999999998</v>
+        <v>1452.922</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="1:10" ht="16" thickBot="1">
-      <c r="A58" s="9"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="7"/>
+    <row r="58" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G58" s="8">
+        <v>2350.4319999999998</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="60" spans="1:10" ht="15" thickBot="1"/>
-    <row r="61" spans="1:10" ht="16" thickBot="1">
-      <c r="A61" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-    </row>
-    <row r="62" spans="1:10" ht="16" thickBot="1">
-      <c r="A62" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" s="13" t="s">
+    <row r="59" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="9"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>150</v>
       </c>
       <c r="D62" s="22"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="13"/>
+      <c r="H62" s="11"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
     </row>
-    <row r="63" spans="1:10" ht="16" thickBot="1">
+    <row r="63" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="13"/>
@@ -2744,15 +2795,15 @@
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
     </row>
-    <row r="64" spans="1:10" ht="16" thickBot="1">
+    <row r="64" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="13"/>
@@ -2760,19 +2811,17 @@
       <c r="G64" s="8"/>
       <c r="H64" s="13"/>
       <c r="I64" s="8"/>
-      <c r="J64" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="16" thickBot="1">
+      <c r="J64" s="8"/>
+    </row>
+    <row r="65" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="13"/>
@@ -2780,17 +2829,19 @@
       <c r="G65" s="8"/>
       <c r="H65" s="13"/>
       <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-    </row>
-    <row r="66" spans="1:10" ht="16" thickBot="1">
+      <c r="J65" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="13"/>
@@ -2800,33 +2851,33 @@
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
     </row>
-    <row r="67" spans="1:10" ht="16" thickBot="1">
-      <c r="A67" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>153</v>
+    <row r="67" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="D67" s="22"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="16"/>
+      <c r="H67" s="13"/>
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
     </row>
-    <row r="68" spans="1:10" ht="16" thickBot="1">
+    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D68" s="22"/>
       <c r="E68" s="16"/>
@@ -2836,48 +2887,67 @@
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
     </row>
-    <row r="69" spans="1:10" ht="15.5">
-      <c r="A69" s="19"/>
+    <row r="69" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+    </row>
+    <row r="70" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A70" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:J58"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A129726C-7E62-40BB-A008-C28D27274ACE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
         <v>154</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>155</v>
       </c>
-      <c r="C1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
+    </row>
+    <row r="2" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>26</v>
@@ -2889,9 +2959,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2903,9 +2973,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4">
         <v>198</v>
@@ -2917,9 +2987,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1">
+    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5">
         <v>213</v>
@@ -2931,9 +3001,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1">
+    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <v>230</v>
@@ -2945,9 +3015,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>236</v>
@@ -2959,9 +3029,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1">
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B8">
         <v>255</v>

</xml_diff>

<commit_message>
Inventor imports for demo buildup
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{8EB54618-A9BB-4D9F-B718-919B5A5B986A}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="6_{5EC64329-1BEC-4FBA-B5CE-250A1E821E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="42" xr10:uidLastSave="{118722B1-5435-443F-800E-960A1741A550}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600" activeTab="1" xr2:uid="{D9AD0EAF-1668-4D2A-B904-AF45542BD22B}"/>
-    <workbookView xWindow="1520" yWindow="0" windowWidth="18060" windowHeight="21600" xr2:uid="{EF99A69C-17B1-4350-A774-B0539ECD671F}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21120" xr2:uid="{EF99A69C-17B1-4350-A774-B0539ECD671F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sum" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="160">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -501,6 +500,12 @@
   </si>
   <si>
     <t>Blue</t>
+  </si>
+  <si>
+    <t>Straight Beams - S4x3</t>
+  </si>
+  <si>
+    <t>S4x3</t>
   </si>
 </sst>
 </file>
@@ -1085,13 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBE6C5D-51A9-46B7-9E2B-F51266F9D3B9}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
@@ -1549,10 +1551,10 @@
     </row>
     <row r="17" spans="1:10" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>158</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>145</v>
@@ -1577,10 +1579,10 @@
     </row>
     <row r="18" spans="1:10" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>145</v>
@@ -1595,7 +1597,7 @@
         <v>141</v>
       </c>
       <c r="G18" s="8">
-        <v>12250.867</v>
+        <v>6365.183</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>141</v>
@@ -1605,10 +1607,10 @@
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>145</v>
@@ -1623,7 +1625,7 @@
         <v>141</v>
       </c>
       <c r="G19" s="8">
-        <v>3040.1970000000001</v>
+        <v>12250.867</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>141</v>
@@ -1633,10 +1635,10 @@
     </row>
     <row r="20" spans="1:10" ht="16" thickBot="1">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>145</v>
@@ -1651,7 +1653,7 @@
         <v>141</v>
       </c>
       <c r="G20" s="8">
-        <v>3036.489</v>
+        <v>3040.1970000000001</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>141</v>
@@ -1661,10 +1663,10 @@
     </row>
     <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>145</v>
@@ -1679,7 +1681,7 @@
         <v>141</v>
       </c>
       <c r="G21" s="8">
-        <v>2158.3809999999999</v>
+        <v>3036.489</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>141</v>
@@ -1689,10 +1691,10 @@
     </row>
     <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>145</v>
@@ -1707,7 +1709,7 @@
         <v>141</v>
       </c>
       <c r="G22" s="8">
-        <v>2137.413</v>
+        <v>2158.3809999999999</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>141</v>
@@ -1717,10 +1719,10 @@
     </row>
     <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>145</v>
@@ -1735,7 +1737,7 @@
         <v>141</v>
       </c>
       <c r="G23" s="8">
-        <v>2588.1860000000001</v>
+        <v>2137.413</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>141</v>
@@ -1745,13 +1747,13 @@
     </row>
     <row r="24" spans="1:10" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>8</v>
@@ -1763,7 +1765,7 @@
         <v>141</v>
       </c>
       <c r="G24" s="8">
-        <v>2351.4119999999998</v>
+        <v>2588.1860000000001</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>141</v>
@@ -1773,10 +1775,10 @@
     </row>
     <row r="25" spans="1:10" ht="16" thickBot="1">
       <c r="A25" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>146</v>
@@ -1791,7 +1793,7 @@
         <v>141</v>
       </c>
       <c r="G25" s="8">
-        <v>3398.395</v>
+        <v>2351.4119999999998</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>141</v>
@@ -1801,16 +1803,16 @@
     </row>
     <row r="26" spans="1:10" ht="16" thickBot="1">
       <c r="A26" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>141</v>
@@ -1819,7 +1821,7 @@
         <v>141</v>
       </c>
       <c r="G26" s="8">
-        <v>829.39300000000003</v>
+        <v>3398.395</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>141</v>
@@ -1829,10 +1831,10 @@
     </row>
     <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>147</v>
@@ -1847,7 +1849,7 @@
         <v>141</v>
       </c>
       <c r="G27" s="8">
-        <v>1271.18</v>
+        <v>829.39300000000003</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>141</v>
@@ -1857,10 +1859,10 @@
     </row>
     <row r="28" spans="1:10" ht="16" thickBot="1">
       <c r="A28" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>147</v>
@@ -1875,7 +1877,7 @@
         <v>141</v>
       </c>
       <c r="G28" s="8">
-        <v>1712.9659999999999</v>
+        <v>1271.18</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>141</v>
@@ -1885,10 +1887,10 @@
     </row>
     <row r="29" spans="1:10" ht="16" thickBot="1">
       <c r="A29" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>147</v>
@@ -1903,7 +1905,7 @@
         <v>141</v>
       </c>
       <c r="G29" s="8">
-        <v>2154.7530000000002</v>
+        <v>1712.9659999999999</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>141</v>
@@ -1913,10 +1915,10 @@
     </row>
     <row r="30" spans="1:10" ht="16" thickBot="1">
       <c r="A30" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>147</v>
@@ -1931,7 +1933,7 @@
         <v>141</v>
       </c>
       <c r="G30" s="8">
-        <v>3921.8980000000001</v>
+        <v>2154.7530000000002</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>141</v>
@@ -1941,10 +1943,10 @@
     </row>
     <row r="31" spans="1:10" ht="16" thickBot="1">
       <c r="A31" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>147</v>
@@ -1959,7 +1961,7 @@
         <v>141</v>
       </c>
       <c r="G31" s="8">
-        <v>5689.0439999999999</v>
+        <v>3921.8980000000001</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>141</v>
@@ -1969,10 +1971,10 @@
     </row>
     <row r="32" spans="1:10" ht="16" thickBot="1">
       <c r="A32" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>147</v>
@@ -1987,7 +1989,7 @@
         <v>141</v>
       </c>
       <c r="G32" s="8">
-        <v>7456.19</v>
+        <v>5689.0439999999999</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>141</v>
@@ -1997,13 +1999,13 @@
     </row>
     <row r="33" spans="1:10" ht="16" thickBot="1">
       <c r="A33" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>78</v>
@@ -2015,7 +2017,7 @@
         <v>141</v>
       </c>
       <c r="G33" s="8">
-        <v>4241.7740000000003</v>
+        <v>7456.19</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>141</v>
@@ -2025,66 +2027,66 @@
     </row>
     <row r="34" spans="1:10" ht="16" thickBot="1">
       <c r="A34" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="17"/>
+        <v>69</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>148</v>
+      </c>
       <c r="D34" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="24" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="G34" s="8">
+        <v>4241.7740000000003</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>137</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="I34" s="8"/>
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="16" thickBot="1">
       <c r="A35" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>149</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C35" s="17"/>
       <c r="D35" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G35" s="8">
-        <v>1312.221</v>
+        <v>143</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="I35" s="8"/>
+        <v>143</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>149</v>
@@ -2099,7 +2101,7 @@
         <v>141</v>
       </c>
       <c r="G36" s="8">
-        <v>3499.375</v>
+        <v>1312.221</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>141</v>
@@ -2109,10 +2111,10 @@
     </row>
     <row r="37" spans="1:10" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>149</v>
@@ -2127,7 +2129,7 @@
         <v>141</v>
       </c>
       <c r="G37" s="8">
-        <v>3493.933</v>
+        <v>3499.375</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>141</v>
@@ -2137,10 +2139,10 @@
     </row>
     <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>149</v>
@@ -2155,7 +2157,7 @@
         <v>141</v>
       </c>
       <c r="G38" s="8">
-        <v>2245.569</v>
+        <v>3493.933</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>141</v>
@@ -2165,13 +2167,13 @@
     </row>
     <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>78</v>
@@ -2183,7 +2185,7 @@
         <v>141</v>
       </c>
       <c r="G39" s="8">
-        <v>387.60700000000003</v>
+        <v>2245.569</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>141</v>
@@ -2193,13 +2195,13 @@
     </row>
     <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>78</v>
@@ -2211,7 +2213,7 @@
         <v>141</v>
       </c>
       <c r="G40" s="8">
-        <v>543.13800000000003</v>
+        <v>387.60700000000003</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>141</v>
@@ -2221,13 +2223,13 @@
     </row>
     <row r="41" spans="1:10" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>78</v>
@@ -2239,7 +2241,7 @@
         <v>141</v>
       </c>
       <c r="G41" s="8">
-        <v>698.66800000000001</v>
+        <v>543.13800000000003</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>141</v>
@@ -2249,31 +2251,41 @@
     </row>
     <row r="42" spans="1:10" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G42" s="8">
+        <v>698.66800000000001</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
     </row>
     <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="7"/>
@@ -2285,38 +2297,28 @@
     </row>
     <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G44" s="8">
-        <v>1227.1959999999999</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>141</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="7"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>149</v>
@@ -2331,7 +2333,7 @@
         <v>141</v>
       </c>
       <c r="G45" s="8">
-        <v>4843.8680000000004</v>
+        <v>1227.1959999999999</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>141</v>
@@ -2341,10 +2343,10 @@
     </row>
     <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>149</v>
@@ -2359,7 +2361,7 @@
         <v>141</v>
       </c>
       <c r="G46" s="8">
-        <v>6677.0190000000002</v>
+        <v>4843.8680000000004</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>141</v>
@@ -2369,10 +2371,10 @@
     </row>
     <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>149</v>
@@ -2387,7 +2389,7 @@
         <v>141</v>
       </c>
       <c r="G47" s="8">
-        <v>5425.3469999999998</v>
+        <v>6677.0190000000002</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>141</v>
@@ -2397,16 +2399,16 @@
     </row>
     <row r="48" spans="1:10" ht="16" thickBot="1">
       <c r="A48" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>141</v>
@@ -2415,7 +2417,7 @@
         <v>141</v>
       </c>
       <c r="G48" s="8">
-        <v>340.899</v>
+        <v>5425.3469999999998</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>141</v>
@@ -2425,10 +2427,10 @@
     </row>
     <row r="49" spans="1:10" ht="16" thickBot="1">
       <c r="A49" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>151</v>
@@ -2443,7 +2445,7 @@
         <v>141</v>
       </c>
       <c r="G49" s="8">
-        <v>480.15</v>
+        <v>340.899</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>141</v>
@@ -2453,10 +2455,10 @@
     </row>
     <row r="50" spans="1:10" ht="16" thickBot="1">
       <c r="A50" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>151</v>
@@ -2471,7 +2473,7 @@
         <v>141</v>
       </c>
       <c r="G50" s="8">
-        <v>418.59699999999998</v>
+        <v>480.15</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>141</v>
@@ -2481,10 +2483,10 @@
     </row>
     <row r="51" spans="1:10" ht="16" thickBot="1">
       <c r="A51" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>151</v>
@@ -2499,7 +2501,7 @@
         <v>141</v>
       </c>
       <c r="G51" s="8">
-        <v>838.15499999999997</v>
+        <v>418.59699999999998</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>141</v>
@@ -2509,10 +2511,10 @@
     </row>
     <row r="52" spans="1:10" ht="16" thickBot="1">
       <c r="A52" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>151</v>
@@ -2527,7 +2529,7 @@
         <v>141</v>
       </c>
       <c r="G52" s="8">
-        <v>1677.269</v>
+        <v>838.15499999999997</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>141</v>
@@ -2537,10 +2539,10 @@
     </row>
     <row r="53" spans="1:10" ht="16" thickBot="1">
       <c r="A53" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>151</v>
@@ -2555,7 +2557,7 @@
         <v>141</v>
       </c>
       <c r="G53" s="8">
-        <v>340.07600000000002</v>
+        <v>1677.269</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>141</v>
@@ -2565,10 +2567,10 @@
     </row>
     <row r="54" spans="1:10" ht="16" thickBot="1">
       <c r="A54" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>151</v>
@@ -2583,7 +2585,7 @@
         <v>141</v>
       </c>
       <c r="G54" s="8">
-        <v>497.10199999999998</v>
+        <v>340.07600000000002</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>141</v>
@@ -2593,10 +2595,10 @@
     </row>
     <row r="55" spans="1:10" ht="16" thickBot="1">
       <c r="A55" s="9" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>151</v>
@@ -2611,25 +2613,23 @@
         <v>141</v>
       </c>
       <c r="G55" s="8">
-        <v>636.35299999999995</v>
+        <v>497.10199999999998</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>141</v>
       </c>
       <c r="I55" s="8"/>
-      <c r="J55" s="8" t="s">
-        <v>136</v>
-      </c>
+      <c r="J55" s="8"/>
     </row>
     <row r="56" spans="1:10" ht="16" thickBot="1">
       <c r="A56" s="9" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>78</v>
@@ -2641,20 +2641,22 @@
         <v>141</v>
       </c>
       <c r="G56" s="8">
-        <v>1452.922</v>
+        <v>636.35299999999995</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>141</v>
       </c>
       <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
+      <c r="J56" s="8" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="57" spans="1:10" ht="16" thickBot="1">
       <c r="A57" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>150</v>
@@ -2669,7 +2671,7 @@
         <v>141</v>
       </c>
       <c r="G57" s="8">
-        <v>2350.4319999999998</v>
+        <v>1452.922</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>141</v>
@@ -2678,60 +2680,70 @@
       <c r="J57" s="8"/>
     </row>
     <row r="58" spans="1:10" ht="16" thickBot="1">
-      <c r="A58" s="9"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="7"/>
+      <c r="A58" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="8">
+        <v>2350.4319999999998</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>141</v>
+      </c>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="60" spans="1:10" ht="15" thickBot="1"/>
-    <row r="61" spans="1:10" ht="16" thickBot="1">
-      <c r="A61" s="10" t="s">
+    <row r="59" spans="1:10" ht="16" thickBot="1">
+      <c r="A59" s="9"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+    </row>
+    <row r="61" spans="1:10" ht="15" thickBot="1"/>
+    <row r="62" spans="1:10" ht="16" thickBot="1">
+      <c r="A62" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B62" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C62" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-    </row>
-    <row r="62" spans="1:10" ht="16" thickBot="1">
-      <c r="A62" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>150</v>
-      </c>
       <c r="D62" s="22"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="13"/>
+      <c r="H62" s="11"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
     </row>
     <row r="63" spans="1:10" ht="16" thickBot="1">
       <c r="A63" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>150</v>
@@ -2746,13 +2758,13 @@
     </row>
     <row r="64" spans="1:10" ht="16" thickBot="1">
       <c r="A64" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="13"/>
@@ -2760,19 +2772,17 @@
       <c r="G64" s="8"/>
       <c r="H64" s="13"/>
       <c r="I64" s="8"/>
-      <c r="J64" s="14" t="s">
-        <v>125</v>
-      </c>
+      <c r="J64" s="8"/>
     </row>
     <row r="65" spans="1:10" ht="16" thickBot="1">
       <c r="A65" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="13"/>
@@ -2780,14 +2790,16 @@
       <c r="G65" s="8"/>
       <c r="H65" s="13"/>
       <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
+      <c r="J65" s="14" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="66" spans="1:10" ht="16" thickBot="1">
       <c r="A66" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>150</v>
@@ -2801,29 +2813,29 @@
       <c r="J66" s="8"/>
     </row>
     <row r="67" spans="1:10" ht="16" thickBot="1">
-      <c r="A67" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>153</v>
+      <c r="A67" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="D67" s="22"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="16"/>
+      <c r="H67" s="13"/>
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
     </row>
     <row r="68" spans="1:10" ht="16" thickBot="1">
       <c r="A68" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>153</v>
@@ -2836,8 +2848,26 @@
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
     </row>
-    <row r="69" spans="1:10" ht="15.5">
-      <c r="A69" s="19"/>
+    <row r="69" spans="1:10" ht="16" thickBot="1">
+      <c r="A69" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.5">
+      <c r="A70" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2849,10 +2879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A129726C-7E62-40BB-A008-C28D27274ACE}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ultrasonic Assembly design added
</commit_message>
<xml_diff>
--- a/Structural parts/Plastic part checklist.xlsx
+++ b/Structural parts/Plastic part checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\RevvyDemoKit\Structural parts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Dani\!_cloud\OneDrive\!_munka\Revolution\RevvyDemoKit\Structural parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_90C2CB4D9809E5910C569C7ADEE56A38BA06B761" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{1E3B455E-A283-4DCF-8C2E-C1E13F8EF08F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="21600"/>
-    <workbookView xWindow="1515" yWindow="0" windowWidth="18060" windowHeight="21600"/>
+    <workbookView xWindow="-14400" yWindow="-6015" windowWidth="14400" windowHeight="8775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sum" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="164">
   <si>
     <t>Plastic Parts</t>
   </si>
@@ -509,13 +509,25 @@
   </si>
   <si>
     <t>Connector Triangle CT2x2</t>
+  </si>
+  <si>
+    <t>CWbA</t>
+  </si>
+  <si>
+    <t>Caster Wheel Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA Battery Pack Case </t>
+  </si>
+  <si>
+    <t>BAcA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,7 +628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -685,17 +697,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -712,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -768,9 +769,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -786,10 +784,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -797,9 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1117,36 +1109,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="21"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
@@ -1154,14 +1143,14 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="31.5" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>142</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1186,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1185,7 @@
       <c r="C3" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -1216,7 +1205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1215,7 @@
       <c r="C4" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1244,7 +1233,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="16" thickBot="1">
       <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +1243,7 @@
       <c r="C5" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1272,7 +1261,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="16" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1271,7 @@
       <c r="C6" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -1300,7 +1289,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
@@ -1310,7 +1299,7 @@
       <c r="C7" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -1328,7 +1317,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1338,7 +1327,7 @@
       <c r="C8" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1356,7 +1345,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1366,7 +1355,7 @@
       <c r="C9" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1384,17 +1373,17 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:10" ht="16" thickBot="1">
+      <c r="A10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1414,7 +1403,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="16" thickBot="1">
       <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
@@ -1424,7 +1413,7 @@
       <c r="C11" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -1442,7 +1431,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
@@ -1452,7 +1441,7 @@
       <c r="C12" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -1470,7 +1459,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
@@ -1480,7 +1469,7 @@
       <c r="C13" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -1498,7 +1487,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1497,7 @@
       <c r="C14" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -1526,7 +1515,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
@@ -1536,7 +1525,7 @@
       <c r="C15" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -1554,7 +1543,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="9" t="s">
         <v>34</v>
       </c>
@@ -1564,7 +1553,7 @@
       <c r="C16" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -1582,7 +1571,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="16" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>157</v>
       </c>
@@ -1592,25 +1581,25 @@
       <c r="C17" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="G17" s="29">
+      <c r="E17" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="8">
         <v>4829.1620000000003</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="27" t="s">
         <v>139</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>36</v>
       </c>
@@ -1620,7 +1609,7 @@
       <c r="C18" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -1638,7 +1627,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="9" t="s">
         <v>38</v>
       </c>
@@ -1648,7 +1637,7 @@
       <c r="C19" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -1666,7 +1655,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="16" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
@@ -1676,7 +1665,7 @@
       <c r="C20" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -1694,7 +1683,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>42</v>
       </c>
@@ -1704,7 +1693,7 @@
       <c r="C21" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -1722,7 +1711,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>44</v>
       </c>
@@ -1732,7 +1721,7 @@
       <c r="C22" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -1750,7 +1739,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>46</v>
       </c>
@@ -1760,7 +1749,7 @@
       <c r="C23" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -1778,17 +1767,17 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:10" ht="16" thickBot="1">
+      <c r="A24" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="7" t="s">
@@ -1808,7 +1797,7 @@
       </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="16" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>50</v>
       </c>
@@ -1818,7 +1807,7 @@
       <c r="C25" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -1836,7 +1825,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="16" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>52</v>
       </c>
@@ -1846,7 +1835,7 @@
       <c r="C26" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -1864,7 +1853,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="9" t="s">
         <v>54</v>
       </c>
@@ -1874,7 +1863,7 @@
       <c r="C27" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -1892,7 +1881,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="16" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>56</v>
       </c>
@@ -1902,7 +1891,7 @@
       <c r="C28" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -1920,7 +1909,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="16" thickBot="1">
       <c r="A29" s="9" t="s">
         <v>58</v>
       </c>
@@ -1930,7 +1919,7 @@
       <c r="C29" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1948,7 +1937,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="16" thickBot="1">
       <c r="A30" s="9" t="s">
         <v>60</v>
       </c>
@@ -1958,7 +1947,7 @@
       <c r="C30" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1976,7 +1965,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="16" thickBot="1">
       <c r="A31" s="9" t="s">
         <v>62</v>
       </c>
@@ -1986,7 +1975,7 @@
       <c r="C31" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -2004,7 +1993,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="16" thickBot="1">
       <c r="A32" s="9" t="s">
         <v>64</v>
       </c>
@@ -2014,7 +2003,7 @@
       <c r="C32" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E32" s="7" t="s">
@@ -2032,7 +2021,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="16" thickBot="1">
       <c r="A33" s="9" t="s">
         <v>66</v>
       </c>
@@ -2042,7 +2031,7 @@
       <c r="C33" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E33" s="7" t="s">
@@ -2060,7 +2049,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="16" thickBot="1">
       <c r="A34" s="9" t="s">
         <v>68</v>
       </c>
@@ -2070,7 +2059,7 @@
       <c r="C34" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -2088,15 +2077,15 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="27" t="s">
+    <row r="35" spans="1:10" ht="16" thickBot="1">
+      <c r="A35" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="22" t="s">
+      <c r="C35" s="26"/>
+      <c r="D35" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -2105,7 +2094,7 @@
       <c r="F35" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="G35" s="23" t="s">
         <v>135</v>
       </c>
       <c r="H35" s="7" t="s">
@@ -2116,17 +2105,17 @@
       </c>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="27" t="s">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
+      <c r="A36" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -2146,7 +2135,7 @@
       </c>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="16" thickBot="1">
       <c r="A37" s="9" t="s">
         <v>159</v>
       </c>
@@ -2156,7 +2145,7 @@
       <c r="C37" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -2174,7 +2163,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="9" t="s">
         <v>72</v>
       </c>
@@ -2184,7 +2173,7 @@
       <c r="C38" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E38" s="7" t="s">
@@ -2202,7 +2191,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="9" t="s">
         <v>74</v>
       </c>
@@ -2212,7 +2201,7 @@
       <c r="C39" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E39" s="7" t="s">
@@ -2230,7 +2219,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="9" t="s">
         <v>76</v>
       </c>
@@ -2240,7 +2229,7 @@
       <c r="C40" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E40" s="7" t="s">
@@ -2258,7 +2247,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="16" thickBot="1">
       <c r="A41" s="9" t="s">
         <v>79</v>
       </c>
@@ -2268,7 +2257,7 @@
       <c r="C41" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E41" s="7" t="s">
@@ -2286,7 +2275,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="16" thickBot="1">
       <c r="A42" s="9" t="s">
         <v>81</v>
       </c>
@@ -2296,7 +2285,7 @@
       <c r="C42" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E42" s="7" t="s">
@@ -2314,17 +2303,17 @@
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="9" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="22"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
@@ -2332,17 +2321,17 @@
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="21"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
@@ -2350,7 +2339,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="9" t="s">
         <v>87</v>
       </c>
@@ -2360,7 +2349,7 @@
       <c r="C45" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
@@ -2378,7 +2367,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="9" t="s">
         <v>89</v>
       </c>
@@ -2388,7 +2377,7 @@
       <c r="C46" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="7" t="s">
@@ -2406,7 +2395,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="9" t="s">
         <v>91</v>
       </c>
@@ -2416,7 +2405,7 @@
       <c r="C47" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="7" t="s">
@@ -2434,7 +2423,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="16" thickBot="1">
       <c r="A48" s="9" t="s">
         <v>93</v>
       </c>
@@ -2444,7 +2433,7 @@
       <c r="C48" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="7" t="s">
@@ -2462,17 +2451,17 @@
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="16" thickBot="1">
       <c r="A49" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E49" s="7" t="s">
@@ -2490,17 +2479,17 @@
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="16" thickBot="1">
       <c r="A50" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="19" t="s">
         <v>98</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="7" t="s">
@@ -2518,7 +2507,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="16" thickBot="1">
       <c r="A51" s="9" t="s">
         <v>99</v>
       </c>
@@ -2528,7 +2517,7 @@
       <c r="C51" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="D51" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E51" s="7" t="s">
@@ -2546,7 +2535,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
     </row>
-    <row r="52" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="16" thickBot="1">
       <c r="A52" s="9" t="s">
         <v>101</v>
       </c>
@@ -2556,7 +2545,7 @@
       <c r="C52" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="22" t="s">
+      <c r="D52" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E52" s="7" t="s">
@@ -2574,7 +2563,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
     </row>
-    <row r="53" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="16" thickBot="1">
       <c r="A53" s="9" t="s">
         <v>103</v>
       </c>
@@ -2584,7 +2573,7 @@
       <c r="C53" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="D53" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E53" s="7" t="s">
@@ -2602,7 +2591,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="16" thickBot="1">
       <c r="A54" s="9" t="s">
         <v>105</v>
       </c>
@@ -2612,7 +2601,7 @@
       <c r="C54" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D54" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E54" s="7" t="s">
@@ -2630,17 +2619,17 @@
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
     </row>
-    <row r="55" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="27" t="s">
+    <row r="55" spans="1:10" ht="16" thickBot="1">
+      <c r="A55" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D55" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E55" s="7" t="s">
@@ -2660,7 +2649,7 @@
       </c>
       <c r="J55" s="8"/>
     </row>
-    <row r="56" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="16" thickBot="1">
       <c r="A56" s="9" t="s">
         <v>132</v>
       </c>
@@ -2670,7 +2659,7 @@
       <c r="C56" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D56" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E56" s="7" t="s">
@@ -2690,7 +2679,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="16" thickBot="1">
       <c r="A57" s="9" t="s">
         <v>109</v>
       </c>
@@ -2700,7 +2689,7 @@
       <c r="C57" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E57" s="7" t="s">
@@ -2718,7 +2707,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
     </row>
-    <row r="58" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="16" thickBot="1">
       <c r="A58" s="9" t="s">
         <v>111</v>
       </c>
@@ -2728,7 +2717,7 @@
       <c r="C58" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E58" s="7" t="s">
@@ -2746,11 +2735,11 @@
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
     </row>
-    <row r="59" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="16" thickBot="1">
       <c r="A59" s="9"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
-      <c r="D59" s="22"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
@@ -2758,8 +2747,8 @@
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
     </row>
-    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15" thickBot="1"/>
+    <row r="62" spans="1:10" ht="16" thickBot="1">
       <c r="A62" s="10" t="s">
         <v>115</v>
       </c>
@@ -2769,7 +2758,7 @@
       <c r="C62" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D62" s="22"/>
+      <c r="D62" s="21"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
       <c r="G62" s="8"/>
@@ -2777,7 +2766,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
     </row>
-    <row r="63" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" ht="16" thickBot="1">
       <c r="A63" s="12" t="s">
         <v>117</v>
       </c>
@@ -2787,7 +2776,7 @@
       <c r="C63" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D63" s="22"/>
+      <c r="D63" s="21"/>
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
       <c r="G63" s="8"/>
@@ -2795,7 +2784,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
     </row>
-    <row r="64" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="16" thickBot="1">
       <c r="A64" s="12" t="s">
         <v>119</v>
       </c>
@@ -2805,7 +2794,7 @@
       <c r="C64" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D64" s="22"/>
+      <c r="D64" s="21"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
       <c r="G64" s="8"/>
@@ -2813,7 +2802,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
     </row>
-    <row r="65" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="16" thickBot="1">
       <c r="A65" s="12" t="s">
         <v>121</v>
       </c>
@@ -2823,7 +2812,7 @@
       <c r="C65" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D65" s="22"/>
+      <c r="D65" s="21"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="G65" s="8"/>
@@ -2833,7 +2822,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="16" thickBot="1">
       <c r="A66" s="12" t="s">
         <v>124</v>
       </c>
@@ -2843,7 +2832,7 @@
       <c r="C66" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D66" s="22"/>
+      <c r="D66" s="21"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
       <c r="G66" s="8"/>
@@ -2851,7 +2840,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
     </row>
-    <row r="67" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" ht="16" thickBot="1">
       <c r="A67" s="12" t="s">
         <v>126</v>
       </c>
@@ -2861,7 +2850,7 @@
       <c r="C67" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="D67" s="22"/>
+      <c r="D67" s="21"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="8"/>
@@ -2869,7 +2858,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
     </row>
-    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="16" thickBot="1">
       <c r="A68" s="15" t="s">
         <v>128</v>
       </c>
@@ -2879,7 +2868,7 @@
       <c r="C68" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="22"/>
+      <c r="D68" s="21"/>
       <c r="E68" s="16"/>
       <c r="F68" s="16"/>
       <c r="G68" s="8"/>
@@ -2887,7 +2876,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
     </row>
-    <row r="69" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="16" thickBot="1">
       <c r="A69" s="15" t="s">
         <v>130</v>
       </c>
@@ -2897,7 +2886,7 @@
       <c r="C69" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D69" s="22"/>
+      <c r="D69" s="21"/>
       <c r="E69" s="16"/>
       <c r="F69" s="16"/>
       <c r="G69" s="8"/>
@@ -2905,33 +2894,87 @@
       <c r="I69" s="8"/>
       <c r="J69" s="8"/>
     </row>
-    <row r="70" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+    <row r="70" spans="1:10" ht="16" thickBot="1">
+      <c r="A70" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="21"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+    </row>
+    <row r="71" spans="1:10" ht="16" thickBot="1">
+      <c r="A71" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+    </row>
+    <row r="72" spans="1:10" ht="16" thickBot="1">
+      <c r="A72" s="12"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+    </row>
+    <row r="73" spans="1:10" ht="16" thickBot="1">
+      <c r="A73" s="12"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J58"/>
+  <autoFilter ref="A2:J58" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -2945,8 +2988,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:4" ht="16" thickBot="1">
+      <c r="A2" s="19" t="s">
         <v>149</v>
       </c>
       <c r="B2">
@@ -2959,7 +3002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>147</v>
       </c>
@@ -2973,7 +3016,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="17" t="s">
         <v>144</v>
       </c>
@@ -2987,7 +3030,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="17" t="s">
         <v>146</v>
       </c>
@@ -3001,7 +3044,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="17" t="s">
         <v>148</v>
       </c>
@@ -3015,7 +3058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="17" t="s">
         <v>145</v>
       </c>
@@ -3029,7 +3072,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="17" t="s">
         <v>143</v>
       </c>

</xml_diff>